<commit_message>
Wrote hardware info and testing software
</commit_message>
<xml_diff>
--- a/Electronic component Stock.xlsx
+++ b/Electronic component Stock.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\ProteusPro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Embedded Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hardware design is finished
</commit_message>
<xml_diff>
--- a/Electronic component Stock.xlsx
+++ b/Electronic component Stock.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Device</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Amount(PCS)</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">CH32V003J4M6 </t>
   </si>
   <si>
@@ -205,6 +202,15 @@
   </si>
   <si>
     <t>5V 4-channel</t>
+  </si>
+  <si>
+    <t>Def</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>3 terminal long</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -493,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -501,13 +507,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -518,13 +524,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -535,10 +541,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E4">
         <v>180</v>
@@ -549,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -560,15 +566,18 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
     </row>
@@ -577,13 +586,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -594,13 +603,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -611,9 +620,12 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
     </row>
@@ -622,7 +634,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -633,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -644,10 +656,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -658,10 +670,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -672,10 +684,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -686,7 +698,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -697,10 +709,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -711,10 +723,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -725,10 +737,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -739,10 +751,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -753,7 +765,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -764,10 +776,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -778,13 +790,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" t="s">
         <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>37</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -795,10 +807,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -809,13 +821,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -826,13 +838,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" t="s">
         <v>43</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
       </c>
       <c r="E25">
         <v>20</v>
@@ -843,13 +855,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>20</v>
@@ -860,13 +872,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27">
         <v>20</v>
@@ -877,13 +889,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28">
         <v>20</v>
@@ -894,13 +906,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29">
         <v>20</v>
@@ -911,10 +923,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -925,10 +937,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31">
         <v>10</v>
@@ -939,10 +951,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32">
         <v>20</v>
@@ -953,10 +965,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -967,13 +979,37 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="4">
         <v>18650</v>
       </c>
       <c r="E34">
         <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>